<commit_message>
Manipulated data and working cat + budget class
</commit_message>
<xml_diff>
--- a/data/Categories.xlsx
+++ b/data/Categories.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Transportation</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Utilities</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Meow</t>
+          <t>Freelance</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rent</t>
         </is>
       </c>
     </row>

</xml_diff>